<commit_message>
Changes to include additional land-use types, etc
</commit_message>
<xml_diff>
--- a/parameters/TransitionCosts/General_conversion.xlsx
+++ b/parameters/TransitionCosts/General_conversion.xlsx
@@ -1,27 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjDir\Africa_Cocoa\trunk\parameters\TransitionCosts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjDir\Luisa_cocoa\parameters\TransitionCosts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{697E3AEF-AAB5-487D-A3A2-86CE32DA47E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6561D3AA-4E45-48F7-8250-7C29DB96E9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
-    <sheet name="exp" sheetId="2" r:id="rId2"/>
+    <sheet name="old" sheetId="3" r:id="rId2"/>
+    <sheet name="exp" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">exp!$A$1:$F$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="90">
   <si>
     <t>Transition</t>
   </si>
@@ -261,12 +278,42 @@
   </si>
   <si>
     <t>Permanent Crops</t>
+  </si>
+  <si>
+    <t>UrbanToNonCompliant_Cocoa</t>
+  </si>
+  <si>
+    <t>NonCompliant_Cocoa</t>
+  </si>
+  <si>
+    <t>UrbanToExhausted_Cocoa</t>
+  </si>
+  <si>
+    <t>Exhausted_Cocoa</t>
+  </si>
+  <si>
+    <t>"FromClass"</t>
+  </si>
+  <si>
+    <t>"ToClass"</t>
+  </si>
+  <si>
+    <t>"cost"</t>
+  </si>
+  <si>
+    <t>"id"</t>
+  </si>
+  <si>
+    <t>"Transition"</t>
+  </si>
+  <si>
+    <t>Overwrite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -805,9 +852,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -845,7 +892,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -951,7 +998,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1093,18 +1140,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection sqref="A1:F65"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,6 +1188,9 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
       <c r="J1" t="s">
         <v>78</v>
       </c>
@@ -1179,6 +1229,10 @@
       <c r="F2">
         <v>-1000</v>
       </c>
+      <c r="G2">
+        <f>VLOOKUP(A2,old!$B$2:$F$65,5,FALSE)</f>
+        <v>-1000</v>
+      </c>
       <c r="J2" t="s">
         <v>7</v>
       </c>
@@ -1217,6 +1271,10 @@
       <c r="F3">
         <v>1000</v>
       </c>
+      <c r="G3">
+        <f>VLOOKUP(A3,old!$B$2:$F$65,5,FALSE)</f>
+        <v>1000</v>
+      </c>
       <c r="J3" t="s">
         <v>9</v>
       </c>
@@ -1255,6 +1313,10 @@
       <c r="F4">
         <v>1000</v>
       </c>
+      <c r="G4">
+        <f>VLOOKUP(A4,old!$B$2:$F$65,5,FALSE)</f>
+        <v>1000</v>
+      </c>
       <c r="J4" t="s">
         <v>79</v>
       </c>
@@ -1293,6 +1355,10 @@
       <c r="F5">
         <v>1000</v>
       </c>
+      <c r="G5">
+        <f>VLOOKUP(A5,old!$B$2:$F$65,5,FALSE)</f>
+        <v>1000</v>
+      </c>
       <c r="J5" t="s">
         <v>13</v>
       </c>
@@ -1331,6 +1397,10 @@
       <c r="F6">
         <v>1000</v>
       </c>
+      <c r="G6">
+        <f>VLOOKUP(A6,old!$B$2:$F$65,5,FALSE)</f>
+        <v>1000</v>
+      </c>
       <c r="J6" t="s">
         <v>21</v>
       </c>
@@ -1369,6 +1439,10 @@
       <c r="F7">
         <v>1000</v>
       </c>
+      <c r="G7">
+        <f>VLOOKUP(A7,old!$B$2:$F$65,5,FALSE)</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1389,6 +1463,10 @@
       <c r="F8">
         <v>1000</v>
       </c>
+      <c r="G8">
+        <f>VLOOKUP(A8,old!$B$2:$F$65,5,FALSE)</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1409,6 +1487,10 @@
       <c r="F9">
         <v>1000</v>
       </c>
+      <c r="G9">
+        <f>VLOOKUP(A9,old!$B$2:$F$65,5,FALSE)</f>
+        <v>1000</v>
+      </c>
       <c r="K9" t="s">
         <v>7</v>
       </c>
@@ -1453,6 +1535,10 @@
       <c r="F10">
         <v>128.66300000000001</v>
       </c>
+      <c r="G10">
+        <f>VLOOKUP(A10,old!$B$2:$F$65,5,FALSE)</f>
+        <v>133.405</v>
+      </c>
       <c r="J10" t="s">
         <v>7</v>
       </c>
@@ -1481,11 +1567,11 @@
         <v>1000</v>
       </c>
       <c r="Q10">
-        <f>N2</f>
+        <f t="shared" ref="Q10:R12" si="1">N2</f>
         <v>1000</v>
       </c>
       <c r="R10">
-        <f>O2</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
     </row>
@@ -1508,6 +1594,10 @@
       <c r="F11">
         <v>-408.084</v>
       </c>
+      <c r="G11">
+        <f>VLOOKUP(A11,old!$B$2:$F$65,5,FALSE)</f>
+        <v>-166.84299999999999</v>
+      </c>
       <c r="J11" t="s">
         <v>9</v>
       </c>
@@ -1536,11 +1626,11 @@
         <v>452.11</v>
       </c>
       <c r="Q11">
-        <f>N3</f>
+        <f t="shared" si="1"/>
         <v>452.11</v>
       </c>
       <c r="R11">
-        <f>O3</f>
+        <f t="shared" si="1"/>
         <v>330.81799999999998</v>
       </c>
     </row>
@@ -1563,6 +1653,10 @@
       <c r="F12">
         <v>358.92099999999999</v>
       </c>
+      <c r="G12">
+        <f>VLOOKUP(A12,old!$B$2:$F$65,5,FALSE)</f>
+        <v>187.185</v>
+      </c>
       <c r="J12" t="s">
         <v>11</v>
       </c>
@@ -1591,11 +1685,11 @@
         <v>462.34100000000001</v>
       </c>
       <c r="Q12">
-        <f>N4</f>
+        <f t="shared" si="1"/>
         <v>462.34100000000001</v>
       </c>
       <c r="R12">
-        <f>O4</f>
+        <f t="shared" si="1"/>
         <v>487.30399999999997</v>
       </c>
     </row>
@@ -1618,6 +1712,10 @@
       <c r="F13">
         <v>452.11</v>
       </c>
+      <c r="G13">
+        <f>VLOOKUP(A13,old!$B$2:$F$65,5,FALSE)</f>
+        <v>168.49799999999999</v>
+      </c>
       <c r="J13" t="s">
         <v>13</v>
       </c>
@@ -1673,6 +1771,10 @@
       <c r="F14">
         <v>452.11</v>
       </c>
+      <c r="G14">
+        <f>VLOOKUP(A14,old!$B$2:$F$65,5,FALSE)</f>
+        <v>168.49799999999999</v>
+      </c>
       <c r="J14" t="s">
         <v>15</v>
       </c>
@@ -1681,11 +1783,11 @@
         <v>289.11</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14:M14" si="1">L5</f>
+        <f t="shared" ref="L14:M14" si="2">L5</f>
         <v>161.13</v>
       </c>
       <c r="M14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>246.898</v>
       </c>
       <c r="N14">
@@ -1726,6 +1828,10 @@
       <c r="F15">
         <v>452.11</v>
       </c>
+      <c r="G15">
+        <f>VLOOKUP(A15,old!$B$2:$F$65,5,FALSE)</f>
+        <v>84.248999999999995</v>
+      </c>
       <c r="J15" t="s">
         <v>17</v>
       </c>
@@ -1734,11 +1840,11 @@
         <v>144.55500000000001</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:R16" si="2">L13/2</f>
+        <f t="shared" ref="L15:R16" si="3">L13/2</f>
         <v>80.564999999999998</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123.449</v>
       </c>
       <c r="N15">
@@ -1757,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.31785</v>
       </c>
     </row>
@@ -1780,6 +1886,10 @@
       <c r="F16">
         <v>452.11</v>
       </c>
+      <c r="G16">
+        <f>VLOOKUP(A16,old!$B$2:$F$65,5,FALSE)</f>
+        <v>84.248999999999995</v>
+      </c>
       <c r="J16" t="s">
         <v>19</v>
       </c>
@@ -1788,11 +1898,11 @@
         <v>144.55500000000001</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80.564999999999998</v>
       </c>
       <c r="M16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123.449</v>
       </c>
       <c r="N16">
@@ -1810,7 +1920,7 @@
         <v>-50</v>
       </c>
       <c r="R16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.31785</v>
       </c>
     </row>
@@ -1833,6 +1943,10 @@
       <c r="F17">
         <v>330.81799999999998</v>
       </c>
+      <c r="G17">
+        <f>VLOOKUP(A17,old!$B$2:$F$65,5,FALSE)</f>
+        <v>257.351</v>
+      </c>
       <c r="J17" t="s">
         <v>21</v>
       </c>
@@ -1841,15 +1955,15 @@
         <v>470.88400000000001</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:N17" si="3">L6</f>
+        <f t="shared" ref="L17:N17" si="4">L6</f>
         <v>83.715100000000007</v>
       </c>
       <c r="M17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27.252700000000001</v>
       </c>
       <c r="N17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>422.30099999999999</v>
       </c>
       <c r="O17">
@@ -1888,6 +2002,10 @@
       <c r="F18">
         <v>364.57100000000003</v>
       </c>
+      <c r="G18">
+        <f>VLOOKUP(A18,old!$B$2:$F$65,5,FALSE)</f>
+        <v>28.032900000000001</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1908,6 +2026,10 @@
       <c r="F19">
         <v>269.483</v>
       </c>
+      <c r="G19">
+        <f>VLOOKUP(A19,old!$B$2:$F$65,5,FALSE)</f>
+        <v>108.011</v>
+      </c>
       <c r="K19" t="s">
         <v>7</v>
       </c>
@@ -1952,6 +2074,10 @@
       <c r="F20">
         <v>-396.24299999999999</v>
       </c>
+      <c r="G20">
+        <f>VLOOKUP(A20,old!$B$2:$F$65,5,FALSE)</f>
+        <v>-55.638399999999997</v>
+      </c>
       <c r="J20" t="s">
         <v>7</v>
       </c>
@@ -1999,6 +2125,10 @@
       <c r="F21">
         <v>462.34100000000001</v>
       </c>
+      <c r="G21">
+        <f>VLOOKUP(A21,old!$B$2:$F$65,5,FALSE)</f>
+        <v>226.19200000000001</v>
+      </c>
       <c r="J21" t="s">
         <v>9</v>
       </c>
@@ -2046,6 +2176,10 @@
       <c r="F22">
         <v>462.34100000000001</v>
       </c>
+      <c r="G22">
+        <f>VLOOKUP(A22,old!$B$2:$F$65,5,FALSE)</f>
+        <v>226.19200000000001</v>
+      </c>
       <c r="J22" t="s">
         <v>11</v>
       </c>
@@ -2093,6 +2227,10 @@
       <c r="F23">
         <v>462.34100000000001</v>
       </c>
+      <c r="G23">
+        <f>VLOOKUP(A23,old!$B$2:$F$65,5,FALSE)</f>
+        <v>113.096</v>
+      </c>
       <c r="J23" t="s">
         <v>13</v>
       </c>
@@ -2140,6 +2278,10 @@
       <c r="F24">
         <v>462.34100000000001</v>
       </c>
+      <c r="G24">
+        <f>VLOOKUP(A24,old!$B$2:$F$65,5,FALSE)</f>
+        <v>113.096</v>
+      </c>
       <c r="J24" t="s">
         <v>15</v>
       </c>
@@ -2187,6 +2329,10 @@
       <c r="F25">
         <v>487.30399999999997</v>
       </c>
+      <c r="G25">
+        <f>VLOOKUP(A25,old!$B$2:$F$65,5,FALSE)</f>
+        <v>8.5359700000000007</v>
+      </c>
       <c r="J25" t="s">
         <v>17</v>
       </c>
@@ -2234,6 +2380,10 @@
       <c r="F26">
         <v>289.11</v>
       </c>
+      <c r="G26">
+        <f>VLOOKUP(A26,old!$B$2:$F$65,5,FALSE)</f>
+        <v>141.53100000000001</v>
+      </c>
       <c r="J26" t="s">
         <v>19</v>
       </c>
@@ -2281,6 +2431,10 @@
       <c r="F27">
         <v>161.13</v>
       </c>
+      <c r="G27">
+        <f>VLOOKUP(A27,old!$B$2:$F$65,5,FALSE)</f>
+        <v>157.25700000000001</v>
+      </c>
       <c r="J27" t="s">
         <v>21</v>
       </c>
@@ -2328,6 +2482,10 @@
       <c r="F28">
         <v>246.898</v>
       </c>
+      <c r="G28">
+        <f>VLOOKUP(A28,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47.2789</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2348,6 +2506,10 @@
       <c r="F29">
         <v>-25.974399999999999</v>
       </c>
+      <c r="G29">
+        <f>VLOOKUP(A29,old!$B$2:$F$65,5,FALSE)</f>
+        <v>-305.80200000000002</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -2368,6 +2530,10 @@
       <c r="F30">
         <v>0</v>
       </c>
+      <c r="G30">
+        <f>VLOOKUP(A30,old!$B$2:$F$65,5,FALSE)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2388,6 +2554,10 @@
       <c r="F31">
         <v>0</v>
       </c>
+      <c r="G31">
+        <f>VLOOKUP(A31,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2408,8 +2578,12 @@
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <f>VLOOKUP(A32,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2428,8 +2602,12 @@
       <c r="F33">
         <v>22.6357</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <f>VLOOKUP(A33,old!$B$2:$F$65,5,FALSE)</f>
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -2448,8 +2626,12 @@
       <c r="F34">
         <v>289.11</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f>VLOOKUP(A34,old!$B$2:$F$65,5,FALSE)</f>
+        <v>141.53100000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -2468,8 +2650,12 @@
       <c r="F35">
         <v>161.13</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <f>VLOOKUP(A35,old!$B$2:$F$65,5,FALSE)</f>
+        <v>157.25700000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -2488,8 +2674,12 @@
       <c r="F36">
         <v>246.898</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f>VLOOKUP(A36,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47.2789</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -2508,8 +2698,12 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <f>VLOOKUP(A37,old!$B$2:$F$65,5,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -2528,8 +2722,12 @@
       <c r="F38">
         <v>-25.974399999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <f>VLOOKUP(A38,old!$B$2:$F$65,5,FALSE)</f>
+        <v>-305.80200000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -2548,8 +2746,12 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <f>VLOOKUP(A39,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -2568,8 +2770,12 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <f>VLOOKUP(A40,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -2588,8 +2794,12 @@
       <c r="F41">
         <v>22.6357</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <f>VLOOKUP(A41,old!$B$2:$F$65,5,FALSE)</f>
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -2608,8 +2818,12 @@
       <c r="F42">
         <v>144.55500000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <f>VLOOKUP(A42,old!$B$2:$F$65,5,FALSE)</f>
+        <v>141.53100000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -2628,8 +2842,12 @@
       <c r="F43">
         <v>80.564999999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <f>VLOOKUP(A43,old!$B$2:$F$65,5,FALSE)</f>
+        <v>157.25700000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -2648,8 +2866,12 @@
       <c r="F44">
         <v>123.449</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <f>VLOOKUP(A44,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47.2789</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -2668,8 +2890,12 @@
       <c r="F45">
         <v>22.6357</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <f>VLOOKUP(A45,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2688,8 +2914,12 @@
       <c r="F46">
         <v>22.6357</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <f>VLOOKUP(A46,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -2708,8 +2938,12 @@
       <c r="F47">
         <v>-50</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <f>VLOOKUP(A47,old!$B$2:$F$65,5,FALSE)</f>
+        <v>-152.90100000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -2728,8 +2962,12 @@
       <c r="F48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <f>VLOOKUP(A48,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -2748,8 +2986,12 @@
       <c r="F49">
         <v>11.31785</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f>VLOOKUP(A49,old!$B$2:$F$65,5,FALSE)</f>
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -2768,8 +3010,12 @@
       <c r="F50">
         <v>144.55500000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <f>VLOOKUP(A50,old!$B$2:$F$65,5,FALSE)</f>
+        <v>141.53100000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -2788,8 +3034,12 @@
       <c r="F51">
         <v>80.564999999999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <f>VLOOKUP(A51,old!$B$2:$F$65,5,FALSE)</f>
+        <v>157.25700000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -2808,8 +3058,12 @@
       <c r="F52">
         <v>123.449</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <f>VLOOKUP(A52,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47.2789</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -2828,8 +3082,12 @@
       <c r="F53">
         <v>22.6357</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <f>VLOOKUP(A53,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -2848,8 +3106,12 @@
       <c r="F54">
         <v>22.6357</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <f>VLOOKUP(A54,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -2868,8 +3130,12 @@
       <c r="F55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <f>VLOOKUP(A55,old!$B$2:$F$65,5,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -2888,8 +3154,12 @@
       <c r="F56">
         <v>-50</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <f>VLOOKUP(A56,old!$B$2:$F$65,5,FALSE)</f>
+        <v>-152.90100000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -2908,8 +3178,12 @@
       <c r="F57">
         <v>11.31785</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <f>VLOOKUP(A57,old!$B$2:$F$65,5,FALSE)</f>
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -2928,8 +3202,12 @@
       <c r="F58">
         <v>470.88400000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <f>VLOOKUP(A58,old!$B$2:$F$65,5,FALSE)</f>
+        <v>429.11700000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -2948,8 +3226,12 @@
       <c r="F59">
         <v>83.715100000000007</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <f>VLOOKUP(A59,old!$B$2:$F$65,5,FALSE)</f>
+        <v>293.34699999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -2968,8 +3250,12 @@
       <c r="F60">
         <v>27.252700000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <f>VLOOKUP(A60,old!$B$2:$F$65,5,FALSE)</f>
+        <v>214.922</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -2988,8 +3274,12 @@
       <c r="F61">
         <v>422.30099999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <f>VLOOKUP(A61,old!$B$2:$F$65,5,FALSE)</f>
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -3008,8 +3298,12 @@
       <c r="F62">
         <v>422.30099999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <f>VLOOKUP(A62,old!$B$2:$F$65,5,FALSE)</f>
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -3028,8 +3322,12 @@
       <c r="F63">
         <v>211.15049999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <f>VLOOKUP(A63,old!$B$2:$F$65,5,FALSE)</f>
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -3048,8 +3346,12 @@
       <c r="F64">
         <v>211.15049999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <f>VLOOKUP(A64,old!$B$2:$F$65,5,FALSE)</f>
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -3067,6 +3369,10 @@
       </c>
       <c r="F65">
         <v>-168.553</v>
+      </c>
+      <c r="G65">
+        <f>VLOOKUP(A65,old!$B$2:$F$65,5,FALSE)</f>
+        <v>-112.892</v>
       </c>
     </row>
   </sheetData>
@@ -3075,17 +3381,1343 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70317C3-77C4-45F4-975F-22A4C8A300A4}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>-1000</v>
+      </c>
+      <c r="F2">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>1000</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1000</v>
+      </c>
+      <c r="F6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>1000</v>
+      </c>
+      <c r="F7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>1000</v>
+      </c>
+      <c r="F8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>1000</v>
+      </c>
+      <c r="F9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>128.66300000000001</v>
+      </c>
+      <c r="F10">
+        <v>133.405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>-408.084</v>
+      </c>
+      <c r="F11">
+        <v>-166.84299999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>358.92099999999999</v>
+      </c>
+      <c r="F12">
+        <v>187.185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>452.11</v>
+      </c>
+      <c r="F13">
+        <v>168.49799999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>452.11</v>
+      </c>
+      <c r="F14">
+        <v>168.49799999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>452.11</v>
+      </c>
+      <c r="F15">
+        <v>84.248999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>452.11</v>
+      </c>
+      <c r="F16">
+        <v>84.248999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>330.81799999999998</v>
+      </c>
+      <c r="F17">
+        <v>257.351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>364.57100000000003</v>
+      </c>
+      <c r="F18">
+        <v>28.032900000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>269.483</v>
+      </c>
+      <c r="F19">
+        <v>108.011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>-396.24299999999999</v>
+      </c>
+      <c r="F20">
+        <v>-55.638399999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21">
+        <v>462.34100000000001</v>
+      </c>
+      <c r="F21">
+        <v>226.19200000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>462.34100000000001</v>
+      </c>
+      <c r="F22">
+        <v>226.19200000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>462.34100000000001</v>
+      </c>
+      <c r="F23">
+        <v>113.096</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24">
+        <v>462.34100000000001</v>
+      </c>
+      <c r="F24">
+        <v>113.096</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25">
+        <v>487.30399999999997</v>
+      </c>
+      <c r="F25">
+        <v>8.5359700000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>289.11</v>
+      </c>
+      <c r="F26">
+        <v>141.53100000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>161.13</v>
+      </c>
+      <c r="F27">
+        <v>157.25700000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>246.898</v>
+      </c>
+      <c r="F28">
+        <v>47.2789</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29">
+        <v>-25.974399999999999</v>
+      </c>
+      <c r="F29">
+        <v>-305.80200000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33">
+        <v>22.6357</v>
+      </c>
+      <c r="F33">
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>289.11</v>
+      </c>
+      <c r="F34">
+        <v>141.53100000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>161.13</v>
+      </c>
+      <c r="F35">
+        <v>157.25700000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>246.898</v>
+      </c>
+      <c r="F36">
+        <v>47.2789</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38">
+        <v>-25.974399999999999</v>
+      </c>
+      <c r="F38">
+        <v>-305.80200000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41">
+        <v>22.6357</v>
+      </c>
+      <c r="F41">
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>144.55500000000001</v>
+      </c>
+      <c r="F42">
+        <v>141.53100000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43">
+        <v>80.564999999999998</v>
+      </c>
+      <c r="F43">
+        <v>157.25700000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44">
+        <v>123.449</v>
+      </c>
+      <c r="F44">
+        <v>47.2789</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45">
+        <v>22.6357</v>
+      </c>
+      <c r="F45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46">
+        <v>22.6357</v>
+      </c>
+      <c r="F46">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47">
+        <v>-50</v>
+      </c>
+      <c r="F47">
+        <v>-152.90100000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49">
+        <v>11.31785</v>
+      </c>
+      <c r="F49">
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>144.55500000000001</v>
+      </c>
+      <c r="F50">
+        <v>141.53100000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51">
+        <v>80.564999999999998</v>
+      </c>
+      <c r="F51">
+        <v>157.25700000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52">
+        <v>123.449</v>
+      </c>
+      <c r="F52">
+        <v>47.2789</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53">
+        <v>22.6357</v>
+      </c>
+      <c r="F53">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54">
+        <v>22.6357</v>
+      </c>
+      <c r="F54">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56">
+        <v>-50</v>
+      </c>
+      <c r="F56">
+        <v>-152.90100000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57">
+        <v>11.31785</v>
+      </c>
+      <c r="F57">
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58">
+        <v>470.88400000000001</v>
+      </c>
+      <c r="F58">
+        <v>429.11700000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59">
+        <v>83.715100000000007</v>
+      </c>
+      <c r="F59">
+        <v>293.34699999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60">
+        <v>27.252700000000001</v>
+      </c>
+      <c r="F60">
+        <v>214.922</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61">
+        <v>422.30099999999999</v>
+      </c>
+      <c r="F61">
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62">
+        <v>422.30099999999999</v>
+      </c>
+      <c r="F62">
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63">
+        <v>211.15049999999999</v>
+      </c>
+      <c r="F63">
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64">
+        <v>211.15049999999999</v>
+      </c>
+      <c r="F64">
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65">
+        <v>-168.553</v>
+      </c>
+      <c r="F65">
+        <v>-112.892</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -3266,1125 +4898,1908 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="F10">
-        <v>128.66300000000001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="F11">
-        <v>-408.084</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F12">
-        <v>358.92099999999999</v>
+        <v>133.405</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F13">
-        <v>452.11</v>
+        <v>-166.84299999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F14">
-        <v>452.11</v>
+        <v>187.185</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F15">
-        <v>452.11</v>
+        <v>168.49799999999999</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F16">
-        <v>452.11</v>
+        <v>168.49799999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F17">
-        <v>330.81799999999998</v>
+        <v>84.248999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F18">
-        <v>364.57100000000003</v>
+        <v>84.248999999999995</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19">
+        <v>257.351</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>D20&amp;"To"&amp;E20</f>
+        <v>CropsToNonCompliant_Cocoa</v>
+      </c>
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19">
-        <v>269.483</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
       <c r="C20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="F20">
-        <v>-396.24299999999999</v>
+        <v>257.351</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>33</v>
+      <c r="A21" t="str">
+        <f>D21&amp;"To"&amp;E21</f>
+        <v>CropsToExhausted_Cocoa</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="F21">
-        <v>462.34100000000001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F22">
-        <v>462.34100000000001</v>
+        <v>28.032900000000001</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F23">
-        <v>462.34100000000001</v>
+        <v>108.011</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F24">
-        <v>462.34100000000001</v>
+        <v>-55.638399999999997</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F25">
-        <v>487.30399999999997</v>
+        <v>226.19200000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F26">
-        <v>289.11</v>
+        <v>226.19200000000001</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F27">
-        <v>161.13</v>
+        <v>113.096</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F28">
-        <v>246.898</v>
+        <v>113.096</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F29">
-        <v>-25.974399999999999</v>
+        <v>8.5359700000000007</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>42</v>
+      <c r="A30" t="str">
+        <f t="shared" ref="A30:A31" si="0">D30&amp;"To"&amp;E30</f>
+        <v>PermanentCropsToNonCompliant_Cocoa</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>8.5359700000000007</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>43</v>
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v>PermanentCropsToExhausted_Cocoa</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>141.53100000000001</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
       <c r="C33">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F33">
-        <v>22.6357</v>
+        <v>157.25700000000001</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F34">
-        <v>289.11</v>
+        <v>47.2789</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F35">
-        <v>161.13</v>
+        <v>-305.80200000000002</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
         <v>4</v>
       </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
       <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
         <v>15</v>
       </c>
-      <c r="E36" t="s">
-        <v>11</v>
-      </c>
       <c r="F36">
-        <v>246.898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F38">
-        <v>-25.974399999999999</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>118.76300000000001</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>52</v>
+      <c r="A40" t="str">
+        <f t="shared" ref="A40:A41" si="1">D40&amp;"To"&amp;E40</f>
+        <v>MatureForestToNonCompliant_Cocoa</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>118.76300000000001</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>53</v>
+      <c r="A41" t="str">
+        <f t="shared" si="1"/>
+        <v>MatureForestToExhausted_Cocoa</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="F41">
-        <v>22.6357</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E42" t="s">
         <v>7</v>
       </c>
       <c r="F42">
-        <v>144.55500000000001</v>
+        <v>141.53100000000001</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
         <v>9</v>
       </c>
       <c r="F43">
-        <v>80.564999999999998</v>
+        <v>157.25700000000001</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
         <v>11</v>
       </c>
       <c r="F44">
-        <v>123.449</v>
+        <v>47.2789</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
       </c>
       <c r="F45">
-        <v>22.6357</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
       </c>
       <c r="F46">
-        <v>22.6357</v>
+        <v>-305.80200000000002</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
         <v>17</v>
       </c>
       <c r="F47">
-        <v>-50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E49" t="s">
         <v>21</v>
       </c>
       <c r="F49">
-        <v>11.31785</v>
+        <v>118.76300000000001</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>62</v>
+      <c r="A50" t="str">
+        <f t="shared" ref="A50:A51" si="2">D50&amp;"To"&amp;E50</f>
+        <v>YoungForestToNonCompliant_Cocoa</v>
       </c>
       <c r="B50">
-        <v>6</v>
+        <f>B49</f>
+        <v>4</v>
       </c>
       <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50" t="s">
-        <v>19</v>
+        <f>C49+1</f>
+        <v>8</v>
+      </c>
+      <c r="D50" t="str">
+        <f>D49</f>
+        <v>YoungForest</v>
       </c>
       <c r="E50" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="F50">
-        <v>144.55500000000001</v>
+        <v>118.76300000000001</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>63</v>
+      <c r="A51" t="str">
+        <f t="shared" si="2"/>
+        <v>YoungForestToExhausted_Cocoa</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <f>B50</f>
+        <v>4</v>
       </c>
       <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>19</v>
+        <f>C50+1</f>
+        <v>9</v>
+      </c>
+      <c r="D51" t="str">
+        <f>D50</f>
+        <v>YoungForest</v>
       </c>
       <c r="E51" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="F51">
-        <v>80.564999999999998</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B52">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F52">
-        <v>123.449</v>
+        <v>141.53100000000001</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B53">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F53">
-        <v>22.6357</v>
+        <v>157.25700000000001</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B54">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F54">
-        <v>22.6357</v>
+        <v>47.2789</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F56">
-        <v>-50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F57">
-        <v>11.31785</v>
+        <v>-152.90100000000001</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F58">
-        <v>470.88400000000001</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B59">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D59" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" t="s">
         <v>21</v>
       </c>
-      <c r="E59" t="s">
-        <v>9</v>
-      </c>
       <c r="F59">
-        <v>83.715100000000007</v>
+        <v>118.76300000000001</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>72</v>
+      <c r="A60" t="str">
+        <f t="shared" ref="A60:A61" si="3">D60&amp;"To"&amp;E60</f>
+        <v>ShrubsToNonCompliant_Cocoa</v>
       </c>
       <c r="B60">
-        <v>7</v>
+        <f>B59</f>
+        <v>5</v>
       </c>
       <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>21</v>
+        <f>C59+1</f>
+        <v>8</v>
+      </c>
+      <c r="D60" t="str">
+        <f>D59</f>
+        <v>Shrubs</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="F60">
-        <v>27.252700000000001</v>
+        <v>118.76300000000001</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>73</v>
+      <c r="A61" t="str">
+        <f t="shared" si="3"/>
+        <v>ShrubsToExhausted_Cocoa</v>
       </c>
       <c r="B61">
-        <v>7</v>
+        <f>B60</f>
+        <v>5</v>
       </c>
       <c r="C61">
-        <v>3</v>
-      </c>
-      <c r="D61" t="s">
-        <v>21</v>
+        <f>C60+1</f>
+        <v>9</v>
+      </c>
+      <c r="D61" t="str">
+        <f>D60</f>
+        <v>Shrubs</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="F61">
-        <v>422.30099999999999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B62">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E62" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F62">
-        <v>422.30099999999999</v>
+        <v>141.53100000000001</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E63" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F63">
-        <v>211.15049999999999</v>
+        <v>157.25700000000001</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E64" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F64">
-        <v>211.15049999999999</v>
+        <v>47.2789</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <v>6</v>
+      </c>
+      <c r="C68">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68">
+        <v>-152.90100000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>6</v>
+      </c>
+      <c r="C69">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" t="s">
+        <v>21</v>
+      </c>
+      <c r="F69">
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="str">
+        <f t="shared" ref="A70:A71" si="4">D70&amp;"To"&amp;E70</f>
+        <v>HerbaceousToNonCompliant_Cocoa</v>
+      </c>
+      <c r="B70">
+        <f>B69</f>
+        <v>6</v>
+      </c>
+      <c r="C70">
+        <f>C69+1</f>
+        <v>8</v>
+      </c>
+      <c r="D70" t="str">
+        <f>D69</f>
+        <v>Herbaceous</v>
+      </c>
+      <c r="E70" t="s">
+        <v>81</v>
+      </c>
+      <c r="F70">
+        <v>118.76300000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="str">
+        <f t="shared" si="4"/>
+        <v>HerbaceousToExhausted_Cocoa</v>
+      </c>
+      <c r="B71">
+        <f>B70</f>
+        <v>6</v>
+      </c>
+      <c r="C71">
+        <f>C70+1</f>
+        <v>9</v>
+      </c>
+      <c r="D71" t="str">
+        <f>D70</f>
+        <v>Herbaceous</v>
+      </c>
+      <c r="E71" t="s">
+        <v>83</v>
+      </c>
+      <c r="F71">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72">
+        <v>429.11700000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73">
+        <v>293.34699999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74">
+        <v>214.922</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>7</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75">
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>7</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" t="s">
+        <v>15</v>
+      </c>
+      <c r="F76">
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+      <c r="C77">
+        <v>5</v>
+      </c>
+      <c r="D77" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F77">
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78">
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="B65">
-        <v>7</v>
-      </c>
-      <c r="C65">
-        <v>7</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="C79">
+        <v>7</v>
+      </c>
+      <c r="D79" t="s">
         <v>21</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E79" t="s">
         <v>21</v>
       </c>
-      <c r="F65">
-        <v>-168.553</v>
+      <c r="F79">
+        <v>-112.892</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="str">
+        <f t="shared" ref="A80:A89" si="5">D80&amp;"To"&amp;E80</f>
+        <v>CocoaToNonCompliant_Cocoa</v>
+      </c>
+      <c r="B80">
+        <f>B79</f>
+        <v>7</v>
+      </c>
+      <c r="C80">
+        <f>C79+1</f>
+        <v>8</v>
+      </c>
+      <c r="D80" t="str">
+        <f>D79</f>
+        <v>Cocoa</v>
+      </c>
+      <c r="E80" t="s">
+        <v>81</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="str">
+        <f t="shared" si="5"/>
+        <v>CocoaToExhausted_Cocoa</v>
+      </c>
+      <c r="B81">
+        <f>B80</f>
+        <v>7</v>
+      </c>
+      <c r="C81">
+        <f>C80+1</f>
+        <v>9</v>
+      </c>
+      <c r="D81" t="str">
+        <f>D80</f>
+        <v>Cocoa</v>
+      </c>
+      <c r="E81" t="s">
+        <v>83</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="str">
+        <f t="shared" si="5"/>
+        <v>NonCompliant_CocoaToUrban</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82">
+        <v>429.11700000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="str">
+        <f t="shared" si="5"/>
+        <v>NonCompliant_CocoaToCrops</v>
+      </c>
+      <c r="B83">
+        <v>8</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>81</v>
+      </c>
+      <c r="E83" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83">
+        <v>293.34699999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f t="shared" si="5"/>
+        <v>NonCompliant_CocoaToPermanentCrops</v>
+      </c>
+      <c r="B84">
+        <v>8</v>
+      </c>
+      <c r="C84">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>81</v>
+      </c>
+      <c r="E84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84">
+        <v>214.922</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="str">
+        <f t="shared" si="5"/>
+        <v>NonCompliant_CocoaToMatureForest</v>
+      </c>
+      <c r="B85">
+        <v>8</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85" t="s">
+        <v>81</v>
+      </c>
+      <c r="E85" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85">
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="str">
+        <f t="shared" si="5"/>
+        <v>NonCompliant_CocoaToYoungForest</v>
+      </c>
+      <c r="B86">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>81</v>
+      </c>
+      <c r="E86" t="s">
+        <v>15</v>
+      </c>
+      <c r="F86">
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="str">
+        <f t="shared" si="5"/>
+        <v>NonCompliant_CocoaToShrubs</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+      <c r="C87">
+        <v>5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" t="s">
+        <v>17</v>
+      </c>
+      <c r="F87">
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
+        <f t="shared" si="5"/>
+        <v>NonCompliant_CocoaToHerbaceous</v>
+      </c>
+      <c r="B88">
+        <v>8</v>
+      </c>
+      <c r="C88">
+        <v>6</v>
+      </c>
+      <c r="D88" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88">
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="str">
+        <f t="shared" si="5"/>
+        <v>NonCompliant_CocoaToCocoa</v>
+      </c>
+      <c r="B89">
+        <v>8</v>
+      </c>
+      <c r="C89">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>81</v>
+      </c>
+      <c r="E89" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="str">
+        <f t="shared" ref="A90:A99" si="6">D90&amp;"To"&amp;E90</f>
+        <v>NonCompliant_CocoaToNonCompliant_Cocoa</v>
+      </c>
+      <c r="B90">
+        <v>8</v>
+      </c>
+      <c r="C90">
+        <f>C89+1</f>
+        <v>8</v>
+      </c>
+      <c r="D90" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" t="s">
+        <v>81</v>
+      </c>
+      <c r="F90">
+        <v>-112.892</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="str">
+        <f t="shared" si="6"/>
+        <v>NonCompliant_CocoaToExhausted_Cocoa</v>
+      </c>
+      <c r="B91">
+        <v>8</v>
+      </c>
+      <c r="C91">
+        <f>C90+1</f>
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>81</v>
+      </c>
+      <c r="E91" t="s">
+        <v>83</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="str">
+        <f t="shared" si="6"/>
+        <v>Exhausted_CocoaToUrban</v>
+      </c>
+      <c r="B92">
+        <v>9</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92" t="s">
+        <v>83</v>
+      </c>
+      <c r="E92" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92">
+        <v>429.11700000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="str">
+        <f t="shared" si="6"/>
+        <v>Exhausted_CocoaToCrops</v>
+      </c>
+      <c r="B93">
+        <v>9</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93">
+        <v>293.34699999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="str">
+        <f t="shared" si="6"/>
+        <v>Exhausted_CocoaToPermanentCrops</v>
+      </c>
+      <c r="B94">
+        <v>9</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
+        <v>83</v>
+      </c>
+      <c r="E94" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94">
+        <v>214.922</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="str">
+        <f t="shared" si="6"/>
+        <v>Exhausted_CocoaToMatureForest</v>
+      </c>
+      <c r="B95">
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>83</v>
+      </c>
+      <c r="E95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95">
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="str">
+        <f t="shared" si="6"/>
+        <v>Exhausted_CocoaToYoungForest</v>
+      </c>
+      <c r="B96">
+        <v>9</v>
+      </c>
+      <c r="C96">
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>83</v>
+      </c>
+      <c r="E96" t="s">
+        <v>15</v>
+      </c>
+      <c r="F96">
+        <v>72.905199999999994</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="str">
+        <f t="shared" si="6"/>
+        <v>Exhausted_CocoaToShrubs</v>
+      </c>
+      <c r="B97">
+        <v>9</v>
+      </c>
+      <c r="C97">
+        <v>5</v>
+      </c>
+      <c r="D97" t="s">
+        <v>83</v>
+      </c>
+      <c r="E97" t="s">
+        <v>17</v>
+      </c>
+      <c r="F97">
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="str">
+        <f t="shared" si="6"/>
+        <v>Exhausted_CocoaToHerbaceous</v>
+      </c>
+      <c r="B98">
+        <v>9</v>
+      </c>
+      <c r="C98">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
+        <v>83</v>
+      </c>
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98">
+        <v>36.452599999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="str">
+        <f t="shared" si="6"/>
+        <v>Exhausted_CocoaToCocoa</v>
+      </c>
+      <c r="B99">
+        <v>9</v>
+      </c>
+      <c r="C99">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
+        <v>83</v>
+      </c>
+      <c r="E99" t="s">
+        <v>21</v>
+      </c>
+      <c r="F99">
+        <v>293.34699999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
+        <f t="shared" ref="A100:A101" si="7">D100&amp;"To"&amp;E100</f>
+        <v>Exhausted_CocoaToNonCompliant_Cocoa</v>
+      </c>
+      <c r="B100">
+        <v>9</v>
+      </c>
+      <c r="C100">
+        <f>C99+1</f>
+        <v>8</v>
+      </c>
+      <c r="D100" t="s">
+        <v>83</v>
+      </c>
+      <c r="E100" t="s">
+        <v>81</v>
+      </c>
+      <c r="F100">
+        <v>293.34699999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="str">
+        <f t="shared" si="7"/>
+        <v>Exhausted_CocoaToExhausted_Cocoa</v>
+      </c>
+      <c r="B101">
+        <v>9</v>
+      </c>
+      <c r="C101">
+        <f>C100+1</f>
+        <v>9</v>
+      </c>
+      <c r="D101" t="s">
+        <v>83</v>
+      </c>
+      <c r="E101" t="s">
+        <v>83</v>
+      </c>
+      <c r="F101">
+        <v>-56.445999999999998</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>